<commit_message>
Updated scrape for diabetes one reciep
</commit_message>
<xml_diff>
--- a/src/test/resources/RecipeExcelData/test.xlsx
+++ b/src/test/resources/RecipeExcelData/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
   <si>
     <t>Recipe ID</t>
   </si>
@@ -25,16 +25,19 @@
     <t>Recipe Category</t>
   </si>
   <si>
+    <t>Ingredients</t>
+  </si>
+  <si>
+    <t>Preparation Time</t>
+  </si>
+  <si>
+    <t>Cooking Time</t>
+  </si>
+  <si>
     <t>Food Category</t>
   </si>
   <si>
-    <t>Ingredients</t>
-  </si>
-  <si>
-    <t>Preparation Time</t>
-  </si>
-  <si>
-    <t>Cooking Time</t>
+    <t>Preparation Method</t>
   </si>
   <si>
     <t>Nutrient values</t>
@@ -44,6 +47,16 @@
   </si>
   <si>
     <t>Recipe URL</t>
+  </si>
+  <si>
+    <t>Recipe# 6409
+04 Jan 19</t>
+  </si>
+  <si>
+    <t>Chawli Bhaji</t>
+  </si>
+  <si>
+    <t>Diabetic recipes recipes</t>
   </si>
   <si>
     <t>8 cups chopped chawli (cow pea / lobhia) leaves
@@ -55,6 +68,43 @@
 4 whole dry kashmiri red chillies , broken into pieces
 2 tsp urad dal (split black lentils)
 a pinch of asafoetida (hing)</t>
+  </si>
+  <si>
+    <t>15 mins</t>
+  </si>
+  <si>
+    <t>11 mins</t>
+  </si>
+  <si>
+    <t>Vegetarian</t>
+  </si>
+  <si>
+    <t>Method
+Combine the chawli leaves, turmeric powder, salt and 1¾ cups of water in a deep non-stick pan and cook on a medium flame for 5 to 7 minutes or till half of the water dries out. Keep aside to cool slightly.
+Blend in a mixer till smooth and keep aside.
+Heat the oil in a non-stick kadhai and add the mustard seeds.
+When the seeds crackle, add the curry leaves, red chillies, urad dal and asafoetida and sauté on a medium flame for a few seconds.
+Add the chawli mixture and a little salt, mix well and cook on a medium flame for 2 to 3 minutes, while stirring occasionally.
+Serve hot.</t>
+  </si>
+  <si>
+    <t>Accompaniments
+Nutritious Lehsuni Methi Roti 
+Nutrient values (Abbrv) per serving
+Energy 91 cal
+Protein 5.9 g
+Carbohydrates 9.5 g
+Fiber 5.7 g
+Fat 3.2 g
+Cholesterol 0 mg
+Sodium 313.6 mg
+Click here to view calories for Chawli Bhaji</t>
+  </si>
+  <si>
+    <t>Diabetes</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/chawli-bhaji-6409r</t>
   </si>
 </sst>
 </file>
@@ -310,7 +360,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -347,10 +397,43 @@
       <c r="J1" t="s" s="0">
         <v>9</v>
       </c>
+      <c r="K1" t="s" s="0">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>14</v>
+      </c>
       <c r="E2" t="s" s="0">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>